<commit_message>
Sorry, benahi test case name
</commit_message>
<xml_diff>
--- a/Test Case.xlsx
+++ b/Test Case.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Register to mobipaid (valid data)</t>
   </si>
   <si>
-    <t xml:space="preserve">Register using valid data without provide optional province</t>
+    <t xml:space="preserve">Register using valid data</t>
   </si>
   <si>
     <t xml:space="preserve">Positif</t>
@@ -77,6 +77,9 @@
   <si>
     <t xml:space="preserve">Register success
 Notice Account successfully activated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register using valid data without provide optional province</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
@@ -301,10 +304,10 @@
   <dimension ref="A1:Z960"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.88"/>
@@ -405,16 +408,16 @@
     <row r="3" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
@@ -440,23 +443,23 @@
     </row>
     <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -481,18 +484,18 @@
     <row r="5" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -520,7 +523,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
@@ -547,16 +550,18 @@
     <row r="7" customFormat="false" ht="243.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -581,12 +586,14 @@
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>

</xml_diff>

<commit_message>
Benahi test case name
</commit_message>
<xml_diff>
--- a/Test Case.xlsx
+++ b/Test Case.xlsx
@@ -79,7 +79,7 @@
 Notice Account successfully activated</t>
   </si>
   <si>
-    <t xml:space="preserve">Register using valid data without provide optional province</t>
+    <t xml:space="preserve">Register using valid data with provide optional province</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
@@ -303,11 +303,11 @@
   </sheetPr>
   <dimension ref="A1:Z960"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.88"/>

</xml_diff>